<commit_message>
commit @20200605 storage newest push.
</commit_message>
<xml_diff>
--- a/KINGKONG_KP_PS_OS_A01/Kingkong_Board_FW_Architecture_A01_20190804.xlsx
+++ b/KINGKONG_KP_PS_OS_A01/Kingkong_Board_FW_Architecture_A01_20190804.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="109">
   <si>
     <t>Test Item</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -376,10 +376,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Fo_St</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>CalRd</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -542,6 +538,17 @@
   <si>
     <t>Tm_Rd:xx.1Celsius OK</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fo_St</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fo_Rd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vo_Rd</t>
   </si>
 </sst>
 </file>
@@ -1138,8 +1145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1180,10 +1187,10 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>6</v>
@@ -1209,7 +1216,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>35</v>
@@ -1232,7 +1239,7 @@
         <v>37</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D5" s="28" t="s">
         <v>45</v>
@@ -1255,7 +1262,7 @@
         <v>38</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D6" s="28" t="s">
         <v>39</v>
@@ -1289,7 +1296,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>18</v>
@@ -1310,7 +1317,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>14</v>
@@ -1331,7 +1338,7 @@
         <v>16</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D10" s="29" t="s">
         <v>19</v>
@@ -1354,7 +1361,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>48</v>
@@ -1377,10 +1384,10 @@
         <v>10</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E12" s="18" t="s">
         <v>22</v>
@@ -1411,16 +1418,16 @@
         <v>26</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E14" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="F14" s="18" t="s">
         <v>87</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>88</v>
       </c>
       <c r="G14" s="18"/>
       <c r="H14" s="2"/>
@@ -1432,16 +1439,16 @@
         <v>26</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D15" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="F15" s="18" t="s">
         <v>89</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="F15" s="18" t="s">
-        <v>90</v>
       </c>
       <c r="G15" s="18"/>
       <c r="H15" s="2"/>
@@ -1453,16 +1460,16 @@
         <v>26</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E16" s="18" t="s">
         <v>67</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G16" s="18"/>
       <c r="H16" s="2"/>
@@ -1474,16 +1481,16 @@
         <v>26</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>68</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G17" s="18"/>
       <c r="H17" s="2"/>
@@ -1495,7 +1502,7 @@
         <v>26</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D18" s="19" t="s">
         <v>66</v>
@@ -1504,7 +1511,7 @@
         <v>69</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G18" s="18"/>
       <c r="H18" s="2"/>
@@ -1516,16 +1523,16 @@
         <v>26</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D19" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="18" t="s">
-        <v>75</v>
-      </c>
       <c r="F19" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G19" s="18"/>
       <c r="H19" s="2"/>
@@ -1537,16 +1544,16 @@
         <v>42</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D20" s="19" t="s">
         <v>65</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G20" s="18"/>
       <c r="H20" s="2"/>
@@ -1558,16 +1565,16 @@
         <v>51</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>71</v>
+        <v>106</v>
       </c>
       <c r="E21" s="19" t="s">
         <v>70</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G21" s="18"/>
       <c r="H21" s="2"/>
@@ -1579,13 +1586,13 @@
         <v>26</v>
       </c>
       <c r="C22" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="E22" s="19" t="s">
         <v>101</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>102</v>
       </c>
       <c r="F22" s="19"/>
       <c r="G22" s="18"/>
@@ -1609,16 +1616,16 @@
         <v>26</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F24" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G24" s="18"/>
       <c r="H24" s="2"/>
@@ -1630,16 +1637,16 @@
         <v>26</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G25" s="18"/>
       <c r="H25" s="2"/>
@@ -1690,7 +1697,9 @@
     <row r="29" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="27"/>
-      <c r="D29" s="2"/>
+      <c r="D29" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
@@ -1701,7 +1710,9 @@
     <row r="30" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="27"/>
-      <c r="D30" s="2"/>
+      <c r="D30" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>

</xml_diff>